<commit_message>
Register user Test Suit has been finished
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramingProjects\KatalonProjects\AcademiaQA_Katalon_YourStoreSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF77134-B481-4C4B-8611-C4775E050CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2273B515-6B4B-44C1-B9B8-668F6BFBA11D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{E828D7EE-574E-4891-A092-A3D3FC4A54AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E828D7EE-574E-4891-A092-A3D3FC4A54AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -117,69 +117,12 @@
     <t>YS-3</t>
   </si>
   <si>
-    <t>Validar el mensaje de error cuando se intenta el registro de un usuario sin Nombre</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de error cuando se intenta registrar un usuario sin Nombre</t>
-  </si>
-  <si>
-    <t>Llenar los datos del formulario para un usuario sin Nombre</t>
-  </si>
-  <si>
     <t>Ver el mensaje de registro fallido por que el usuario no tiene el dato Nombre</t>
   </si>
   <si>
     <t>YS-4</t>
   </si>
   <si>
-    <t>YS-5</t>
-  </si>
-  <si>
-    <t>YS-6</t>
-  </si>
-  <si>
-    <t>YS-7</t>
-  </si>
-  <si>
-    <t>Validar el mensaje de error cuando se intenta el registro de un usuario sin Apellido</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de error cuando se intenta registrar un usuario sin Apellido</t>
-  </si>
-  <si>
-    <t>Llenar los datos del formulario para un usuario sin Apellido</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de registro fallido por que el usuario no tiene el dato Apellido</t>
-  </si>
-  <si>
-    <t>Validar el mensaje de error cuando se intenta el registro de un usuario sin Telefono</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de error cuando se intenta registrar un usuario sin Telefono</t>
-  </si>
-  <si>
-    <t>Llenar los datos del formulario para un usuario sin Telefono</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de registro fallido por que el usuario no tiene el dato Telefono</t>
-  </si>
-  <si>
-    <t>YS-8</t>
-  </si>
-  <si>
-    <t>Validar el mensaje de error cuando se intenta el registro de un usuario sin Contraseña</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de error cuando se intenta registrar un usuario sin Contraseña</t>
-  </si>
-  <si>
-    <t>Llenar los datos del formulario para un usuario sin Contraseña</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de registro fallido por que el usuario no tiene el dato Contraseña</t>
-  </si>
-  <si>
     <t>Validar el mensaje de error cuando se intenta el registro de un usuario sin Politicas de Privacidad</t>
   </si>
   <si>
@@ -189,16 +132,13 @@
     <t>Ver el mensaje de registro fallido por que el usuario no tiene el dato Politicas de Privacidad</t>
   </si>
   <si>
-    <t>Validar el mensaje de error cuando se intenta el registro de un usuario sin Correo Electrónico</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de error cuando se intenta registrar un usuario sin Correo Electrónico</t>
-  </si>
-  <si>
-    <t>Llenar los datos del formulario para un usuario sin Correo Electrónico</t>
-  </si>
-  <si>
-    <t>Ver el mensaje de registro fallido por que el usuario no tiene el dato Correo Electrónico</t>
+    <t>Validar el mensaje de error cuando se intenta el registro de un usuario sin un Parametro</t>
+  </si>
+  <si>
+    <t>Ver el mensaje de error cuando se intenta registrar un usuario sin un Parametro</t>
+  </si>
+  <si>
+    <t>Llenar los datos del formulario para un usuario sin un Parametro</t>
   </si>
 </sst>
 </file>
@@ -605,17 +545,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F160DA0-27CE-4E13-A4C2-D2168D484335}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
     <col min="6" max="6" width="32.5703125" style="1" customWidth="1"/>
   </cols>
@@ -660,7 +600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -672,7 +612,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -686,7 +626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -696,7 +636,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -730,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -742,7 +682,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -756,7 +696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -785,10 +725,10 @@
         <v>27</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>12</v>
@@ -800,7 +740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -812,12 +752,12 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>17</v>
@@ -826,7 +766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -844,7 +784,7 @@
         <v>25</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>8</v>
@@ -852,13 +792,13 @@
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>12</v>
@@ -870,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -882,12 +822,12 @@
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>17</v>
@@ -896,307 +836,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="E20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="12">
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="A2:A6"/>
@@ -1206,21 +866,9 @@
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>